<commit_message>
Matlab tool to compute KPIs
</commit_message>
<xml_diff>
--- a/templates/default_values.xlsx
+++ b/templates/default_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.barla\Documents\Local_codes\HVDCWISE_TEA.jl\studies\simple_use_case\user_interface\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.barla\Documents\Local_codes\HVDCWISE_TEA.jl\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9724F6C1-0D80-433A-9E34-D15AD9AF1858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AD3722-2AC9-471D-BA02-13ACE40A2CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="585" windowWidth="15000" windowHeight="14865" tabRatio="743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="16005" windowHeight="10335" tabRatio="743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="16" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="201">
   <si>
     <t>Content</t>
   </si>
@@ -678,13 +678,16 @@
   </si>
   <si>
     <t>For a voltage of 1 pu. G_MW = G_S * V_base². Usually 0.</t>
+  </si>
+  <si>
+    <t>thermal_rating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,12 +724,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1226,10 +1223,10 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C124" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomRight" activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,7 +2326,7 @@
         <v>45</v>
       </c>
       <c r="E66" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2378,7 +2375,7 @@
         <v>45</v>
       </c>
       <c r="E69" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2497,7 +2494,7 @@
         <v>45</v>
       </c>
       <c r="E76" s="24">
-        <v>0</v>
+        <v>0.88700000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3545,15 +3542,15 @@
         <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>185</v>
-      </c>
-      <c r="C141" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="C141" t="s">
+        <v>39</v>
+      </c>
       <c r="D141" t="s">
         <v>45</v>
       </c>
-      <c r="E141" s="24">
-        <v>1</v>
-      </c>
+      <c r="E141" s="23"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
@@ -6212,18 +6209,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
-    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100360305CF8A5F8A4B86568FB88F41EB51" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="7820bdd98b12bbce6701f392baa49827">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xmlns:ns3="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a7208ee71179b2cd86960a83168177e" ns2:_="" ns3:_="">
     <xsd:import namespace="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
@@ -6464,7 +6449,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6473,18 +6458,19 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C116F8E2-4DBC-4DB4-825C-1F8126BA2EE0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
-    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
+    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFB0FD70-63EF-4D48-A8C4-DFC9646D4D60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6503,10 +6489,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FD1144D-069D-4B6F-AEE5-711B319AB663}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C116F8E2-4DBC-4DB4-825C-1F8126BA2EE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
+    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Several economic indicators instead of SEW
</commit_message>
<xml_diff>
--- a/templates/default_values.xlsx
+++ b/templates/default_values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.barla\Documents\Local_codes\HVDCWISE_TEA.jl\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349AA2F7-5377-45D1-8576-83785449E661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523538AE-5873-452C-A588-90A96BE6E694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="16" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="294">
   <si>
     <t>bus</t>
   </si>
@@ -516,9 +516,6 @@
     <t>cost_red</t>
   </si>
   <si>
-    <t xml:space="preserve">cost_curt </t>
-  </si>
-  <si>
     <t>cost_inv</t>
   </si>
   <si>
@@ -544,12 +541,6 @@
   </si>
   <si>
     <t>With base energy = annual load</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.1974</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0.0</t>
   </si>
   <si>
     <t>storage_bus</t>
@@ -982,19 +973,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1547,10 +1532,10 @@
   <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1550,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>12</v>
@@ -1577,7 +1562,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1591,7 +1576,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E2" s="7"/>
     </row>
@@ -1603,7 +1588,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>33</v>
@@ -1623,7 +1608,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E4" s="9">
         <v>0</v>
@@ -1640,7 +1625,7 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E5" s="9">
         <v>0</v>
@@ -1657,7 +1642,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E6" s="9">
         <v>0</v>
@@ -1674,7 +1659,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E7" s="9">
         <v>0</v>
@@ -1691,7 +1676,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E8" s="9">
         <v>1</v>
@@ -1708,7 +1693,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E9" s="9">
         <v>1</v>
@@ -1722,10 +1707,10 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E10" s="9">
         <v>0</v>
@@ -1742,7 +1727,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E11" s="10"/>
     </row>
@@ -1757,7 +1742,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E12" s="9">
         <v>1</v>
@@ -1774,7 +1759,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E13" s="9">
         <v>1.1000000000000001</v>
@@ -1791,7 +1776,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E14" s="13">
         <v>0.9</v>
@@ -1808,7 +1793,7 @@
         <v>27</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E15" s="16"/>
     </row>
@@ -1823,7 +1808,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E16" s="17">
         <v>1</v>
@@ -1840,7 +1825,7 @@
         <v>28</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E17" s="17">
         <v>0</v>
@@ -1857,7 +1842,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E18" s="17">
         <v>1</v>
@@ -1874,7 +1859,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E19" s="16"/>
     </row>
@@ -1889,7 +1874,7 @@
         <v>30</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E20" s="17">
         <v>1.05</v>
@@ -1906,7 +1891,7 @@
         <v>30</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E21" s="17">
         <v>0.95</v>
@@ -1923,7 +1908,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E22" s="17">
         <v>0</v>
@@ -1940,7 +1925,7 @@
         <v>27</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E23" s="15"/>
     </row>
@@ -1955,7 +1940,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E24" s="16"/>
     </row>
@@ -1970,7 +1955,7 @@
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E25" s="16"/>
     </row>
@@ -1985,7 +1970,7 @@
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E26" s="16"/>
     </row>
@@ -2000,7 +1985,7 @@
         <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E27" s="17">
         <v>0</v>
@@ -2017,7 +2002,7 @@
         <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E28" s="16"/>
     </row>
@@ -2032,7 +2017,7 @@
         <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E29" s="27"/>
     </row>
@@ -2047,7 +2032,7 @@
         <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E30" s="27"/>
     </row>
@@ -2062,7 +2047,7 @@
         <v>42</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E31" s="17">
         <v>0</v>
@@ -2076,10 +2061,10 @@
         <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E32" s="17">
         <v>0</v>
@@ -2096,7 +2081,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E33" s="17">
         <v>1</v>
@@ -2110,10 +2095,10 @@
         <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E34" s="17">
         <v>-60</v>
@@ -2127,10 +2112,10 @@
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E35" s="17">
         <v>60</v>
@@ -2144,10 +2129,10 @@
         <v>56</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E36" s="28"/>
     </row>
@@ -2162,7 +2147,7 @@
         <v>27</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E37" s="15"/>
     </row>
@@ -2177,7 +2162,7 @@
         <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E38" s="16"/>
     </row>
@@ -2192,7 +2177,7 @@
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E39" s="16"/>
     </row>
@@ -2204,10 +2189,10 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D40" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E40" s="17">
         <v>0</v>
@@ -2221,10 +2206,10 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D41" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E41" s="17">
         <v>0</v>
@@ -2241,7 +2226,7 @@
         <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E42" s="16"/>
     </row>
@@ -2256,7 +2241,7 @@
         <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E43" s="27"/>
     </row>
@@ -2271,7 +2256,7 @@
         <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E44" s="27"/>
     </row>
@@ -2286,7 +2271,7 @@
         <v>104</v>
       </c>
       <c r="D45" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E45" s="17">
         <v>1</v>
@@ -2300,10 +2285,10 @@
         <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D46" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E46" s="16"/>
     </row>
@@ -2318,7 +2303,7 @@
         <v>121</v>
       </c>
       <c r="D47" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E47" s="17">
         <v>2</v>
@@ -2335,7 +2320,7 @@
         <v>30</v>
       </c>
       <c r="D48" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E48" s="27"/>
     </row>
@@ -2347,10 +2332,10 @@
         <v>65</v>
       </c>
       <c r="C49" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D49" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E49" s="17">
         <v>0</v>
@@ -2367,7 +2352,7 @@
         <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E50" s="17">
         <v>1</v>
@@ -2384,7 +2369,7 @@
         <v>104</v>
       </c>
       <c r="D51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E51" s="17">
         <v>1</v>
@@ -2401,7 +2386,7 @@
         <v>104</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E52" s="19">
         <v>1</v>
@@ -2418,7 +2403,7 @@
         <v>27</v>
       </c>
       <c r="D53" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E53" s="16"/>
     </row>
@@ -2433,7 +2418,7 @@
         <v>27</v>
       </c>
       <c r="D54" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E54" s="16"/>
     </row>
@@ -2445,10 +2430,10 @@
         <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D55" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E55" s="17">
         <v>1</v>
@@ -2462,10 +2447,10 @@
         <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D56" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E56" s="17">
         <v>1</v>
@@ -2482,7 +2467,7 @@
         <v>28</v>
       </c>
       <c r="D57" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E57" s="17">
         <v>0</v>
@@ -2499,7 +2484,7 @@
         <v>29</v>
       </c>
       <c r="D58" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E58" s="17">
         <v>0</v>
@@ -2516,7 +2501,7 @@
         <v>104</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E59" s="17">
         <v>0</v>
@@ -2533,7 +2518,7 @@
         <v>30</v>
       </c>
       <c r="D60" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E60" s="17">
         <v>1</v>
@@ -2550,7 +2535,7 @@
         <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E61" s="27"/>
     </row>
@@ -2565,7 +2550,7 @@
         <v>30</v>
       </c>
       <c r="D62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E62" s="27"/>
     </row>
@@ -2580,7 +2565,7 @@
         <v>104</v>
       </c>
       <c r="D63" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E63" s="17">
         <v>1</v>
@@ -2597,7 +2582,7 @@
         <v>105</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E64" s="17">
         <v>1</v>
@@ -2614,7 +2599,7 @@
         <v>30</v>
       </c>
       <c r="D65" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E65" s="17">
         <v>0</v>
@@ -2631,7 +2616,7 @@
         <v>104</v>
       </c>
       <c r="D66" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E66" s="17">
         <v>0</v>
@@ -2648,7 +2633,7 @@
         <v>30</v>
       </c>
       <c r="D67" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E67" s="27"/>
     </row>
@@ -2663,7 +2648,7 @@
         <v>30</v>
       </c>
       <c r="D68" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E68" s="27"/>
     </row>
@@ -2678,7 +2663,7 @@
         <v>104</v>
       </c>
       <c r="D69" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E69" s="17">
         <v>0</v>
@@ -2695,7 +2680,7 @@
         <v>31</v>
       </c>
       <c r="D70" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E70" s="27"/>
     </row>
@@ -2710,7 +2695,7 @@
         <v>30</v>
       </c>
       <c r="D71" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E71" s="17">
         <v>1.05</v>
@@ -2727,7 +2712,7 @@
         <v>30</v>
       </c>
       <c r="D72" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E72" s="17">
         <v>0.95</v>
@@ -2744,7 +2729,7 @@
         <v>30</v>
       </c>
       <c r="D73" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E73" s="26">
         <v>1.1000000000000001</v>
@@ -2761,7 +2746,7 @@
         <v>104</v>
       </c>
       <c r="D74" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E74" s="17">
         <v>1</v>
@@ -2778,7 +2763,7 @@
         <v>28</v>
       </c>
       <c r="D75" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E75" s="17">
         <v>0</v>
@@ -2795,7 +2780,7 @@
         <v>31</v>
       </c>
       <c r="D76" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E76" s="17">
         <v>0</v>
@@ -2812,7 +2797,7 @@
         <v>106</v>
       </c>
       <c r="D77" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E77" s="17">
         <v>0</v>
@@ -2829,7 +2814,7 @@
         <v>106</v>
       </c>
       <c r="D78" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E78" s="17">
         <v>0</v>
@@ -2843,10 +2828,10 @@
         <v>93</v>
       </c>
       <c r="C79" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D79" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E79" s="17">
         <v>5.0000000000000001E-3</v>
@@ -2863,7 +2848,7 @@
         <v>28</v>
       </c>
       <c r="D80" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E80" s="17">
         <v>0</v>
@@ -2880,7 +2865,7 @@
         <v>30</v>
       </c>
       <c r="D81" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E81" s="17">
         <v>1</v>
@@ -2897,7 +2882,7 @@
         <v>30</v>
       </c>
       <c r="D82" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E82" s="17">
         <v>0</v>
@@ -2914,7 +2899,7 @@
         <v>28</v>
       </c>
       <c r="D83" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E83" s="16"/>
     </row>
@@ -2929,7 +2914,7 @@
         <v>28</v>
       </c>
       <c r="D84" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E84" s="27"/>
     </row>
@@ -2944,7 +2929,7 @@
         <v>29</v>
       </c>
       <c r="D85" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E85" s="27"/>
     </row>
@@ -2959,7 +2944,7 @@
         <v>29</v>
       </c>
       <c r="D86" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E86" s="27"/>
     </row>
@@ -2971,10 +2956,10 @@
         <v>101</v>
       </c>
       <c r="C87" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D87" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E87" s="16"/>
     </row>
@@ -2986,10 +2971,10 @@
         <v>65</v>
       </c>
       <c r="C88" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D88" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E88" s="17">
         <v>0</v>
@@ -3006,7 +2991,7 @@
         <v>104</v>
       </c>
       <c r="D89" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E89" s="17">
         <v>0</v>
@@ -3023,7 +3008,7 @@
         <v>30</v>
       </c>
       <c r="D90" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E90" s="27"/>
     </row>
@@ -3038,7 +3023,7 @@
         <v>104</v>
       </c>
       <c r="D91" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E91" s="17">
         <v>1</v>
@@ -3055,7 +3040,7 @@
         <v>104</v>
       </c>
       <c r="D92" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E92" s="17">
         <v>1</v>
@@ -3063,16 +3048,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D93" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>180</v>
       </c>
       <c r="E93" s="15"/>
     </row>
@@ -3087,7 +3072,7 @@
         <v>27</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E94" s="15"/>
     </row>
@@ -3102,7 +3087,7 @@
         <v>28</v>
       </c>
       <c r="D95" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E95" s="17">
         <v>0</v>
@@ -3119,7 +3104,7 @@
         <v>29</v>
       </c>
       <c r="D96" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E96" s="17">
         <v>0</v>
@@ -3136,7 +3121,7 @@
         <v>29</v>
       </c>
       <c r="D97" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E97" s="17">
         <v>0</v>
@@ -3153,7 +3138,7 @@
         <v>29</v>
       </c>
       <c r="D98" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E98" s="17">
         <v>0</v>
@@ -3170,7 +3155,7 @@
         <v>30</v>
       </c>
       <c r="D99" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E99" s="17">
         <v>0</v>
@@ -3187,7 +3172,7 @@
         <v>55</v>
       </c>
       <c r="D100" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E100" s="17">
         <v>0</v>
@@ -3204,7 +3189,7 @@
         <v>104</v>
       </c>
       <c r="D101" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E101" s="17">
         <v>1</v>
@@ -3221,7 +3206,7 @@
         <v>28</v>
       </c>
       <c r="D102" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E102" s="16"/>
     </row>
@@ -3236,7 +3221,7 @@
         <v>28</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E103" s="19">
         <v>0</v>
@@ -3270,7 +3255,7 @@
         <v>122</v>
       </c>
       <c r="D105" s="23" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E105" s="17">
         <v>0</v>
@@ -3287,7 +3272,7 @@
         <v>122</v>
       </c>
       <c r="D106" s="23" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E106" s="17">
         <v>0</v>
@@ -3304,7 +3289,7 @@
         <v>121</v>
       </c>
       <c r="D107" s="23" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E107" s="17">
         <v>2</v>
@@ -3321,7 +3306,7 @@
         <v>123</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E108" s="16"/>
     </row>
@@ -3336,7 +3321,7 @@
         <v>122</v>
       </c>
       <c r="D109" s="23" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E109" s="17">
         <v>0</v>
@@ -3353,7 +3338,7 @@
         <v>27</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E110" s="15"/>
     </row>
@@ -3368,7 +3353,7 @@
         <v>28</v>
       </c>
       <c r="D111" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E111" s="16"/>
     </row>
@@ -3383,7 +3368,7 @@
         <v>29</v>
       </c>
       <c r="D112" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E112" s="17">
         <v>0</v>
@@ -3400,7 +3385,7 @@
         <v>29</v>
       </c>
       <c r="D113" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E113" s="17">
         <v>0</v>
@@ -3417,7 +3402,7 @@
         <v>104</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E114" s="17">
         <v>1</v>
@@ -3434,7 +3419,7 @@
         <v>123</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E115" s="17">
         <v>0</v>
@@ -3451,7 +3436,7 @@
         <v>123</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E116" s="20"/>
     </row>
@@ -3466,7 +3451,7 @@
         <v>27</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E117" s="16"/>
     </row>
@@ -3478,13 +3463,13 @@
         <v>133</v>
       </c>
       <c r="C118" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D118" s="23" t="s">
-        <v>271</v>
-      </c>
-      <c r="E118" s="17" t="s">
-        <v>153</v>
+        <v>268</v>
+      </c>
+      <c r="E118" s="17">
+        <v>0.19739999999999999</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3495,10 +3480,10 @@
         <v>134</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E119" s="16"/>
     </row>
@@ -3510,10 +3495,10 @@
         <v>135</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E120" s="16"/>
     </row>
@@ -3525,10 +3510,10 @@
         <v>136</v>
       </c>
       <c r="C121" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E121" s="17">
         <v>4</v>
@@ -3542,10 +3527,10 @@
         <v>137</v>
       </c>
       <c r="C122" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E122" s="17">
         <v>4</v>
@@ -3559,10 +3544,10 @@
         <v>138</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E123" s="17">
         <v>0</v>
@@ -3576,10 +3561,10 @@
         <v>139</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E124" s="16"/>
     </row>
@@ -3591,10 +3576,10 @@
         <v>140</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E125" s="17">
         <v>0</v>
@@ -3611,7 +3596,7 @@
         <v>123</v>
       </c>
       <c r="D126" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E126" s="16"/>
     </row>
@@ -3626,7 +3611,7 @@
         <v>123</v>
       </c>
       <c r="D127" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E127" s="16"/>
     </row>
@@ -3635,13 +3620,13 @@
         <v>9</v>
       </c>
       <c r="B128" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C128" t="s">
         <v>123</v>
       </c>
       <c r="D128" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E128" s="16"/>
     </row>
@@ -3650,13 +3635,13 @@
         <v>9</v>
       </c>
       <c r="B129" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D129" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E129" s="26">
         <v>100000</v>
@@ -3667,33 +3652,31 @@
         <v>9</v>
       </c>
       <c r="B130" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C130" t="s">
         <v>104</v>
       </c>
       <c r="D130" s="23" t="s">
-        <v>271</v>
-      </c>
-      <c r="E130" s="17">
-        <v>1</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="E130" s="16"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B131" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D131" s="23" t="s">
-        <v>271</v>
-      </c>
-      <c r="E131" s="17" t="s">
-        <v>154</v>
+        <v>268</v>
+      </c>
+      <c r="E131" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3701,13 +3684,13 @@
         <v>9</v>
       </c>
       <c r="B132" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D132" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E132" s="17">
         <v>10</v>
@@ -3718,13 +3701,13 @@
         <v>10</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C133" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E133" s="15"/>
     </row>
@@ -3733,13 +3716,13 @@
         <v>10</v>
       </c>
       <c r="B134" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C134" t="s">
         <v>28</v>
       </c>
       <c r="D134" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E134" s="17">
         <v>0</v>
@@ -3750,13 +3733,13 @@
         <v>10</v>
       </c>
       <c r="B135" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C135" t="s">
         <v>29</v>
       </c>
       <c r="D135" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E135" s="17">
         <v>0</v>
@@ -3767,13 +3750,13 @@
         <v>10</v>
       </c>
       <c r="B136" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C136" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D136" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E136" s="16"/>
     </row>
@@ -3782,13 +3765,13 @@
         <v>10</v>
       </c>
       <c r="B137" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C137" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D137" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E137" s="16"/>
     </row>
@@ -3797,13 +3780,13 @@
         <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C138" t="s">
         <v>28</v>
       </c>
       <c r="D138" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E138" s="16"/>
     </row>
@@ -3812,13 +3795,13 @@
         <v>10</v>
       </c>
       <c r="B139" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C139" t="s">
         <v>28</v>
       </c>
       <c r="D139" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E139" s="16"/>
     </row>
@@ -3827,13 +3810,13 @@
         <v>10</v>
       </c>
       <c r="B140" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C140" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D140" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E140" s="16"/>
     </row>
@@ -3842,13 +3825,13 @@
         <v>10</v>
       </c>
       <c r="B141" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C141" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D141" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E141" s="16"/>
     </row>
@@ -3857,13 +3840,13 @@
         <v>10</v>
       </c>
       <c r="B142" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
       </c>
       <c r="D142" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E142" s="16"/>
     </row>
@@ -3878,7 +3861,7 @@
         <v>29</v>
       </c>
       <c r="D143" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E143" s="17">
         <v>-1</v>
@@ -3895,7 +3878,7 @@
         <v>29</v>
       </c>
       <c r="D144" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E144" s="17">
         <v>1</v>
@@ -3912,7 +3895,7 @@
         <v>30</v>
       </c>
       <c r="D145" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E145" s="17">
         <v>0</v>
@@ -3929,7 +3912,7 @@
         <v>30</v>
       </c>
       <c r="D146" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E146" s="17">
         <v>0</v>
@@ -3940,13 +3923,13 @@
         <v>10</v>
       </c>
       <c r="B147" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C147" t="s">
         <v>28</v>
       </c>
       <c r="D147" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E147" s="17">
         <v>0</v>
@@ -3957,13 +3940,13 @@
         <v>10</v>
       </c>
       <c r="B148" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C148" t="s">
         <v>29</v>
       </c>
       <c r="D148" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E148" s="17">
         <v>0</v>
@@ -3980,7 +3963,7 @@
         <v>104</v>
       </c>
       <c r="D149" s="18" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E149" s="19">
         <v>1</v>
@@ -3991,13 +3974,13 @@
         <v>11</v>
       </c>
       <c r="B150" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D150" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E150" s="17">
         <v>0</v>
@@ -4008,13 +3991,13 @@
         <v>11</v>
       </c>
       <c r="B151" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C151" t="s">
         <v>30</v>
       </c>
       <c r="D151" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E151" s="17">
         <v>0</v>
@@ -4025,13 +4008,13 @@
         <v>11</v>
       </c>
       <c r="B152" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C152" t="s">
         <v>30</v>
       </c>
       <c r="D152" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E152" s="17">
         <v>0</v>
@@ -4042,13 +4025,13 @@
         <v>11</v>
       </c>
       <c r="B153" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C153" s="22" t="s">
         <v>30</v>
       </c>
       <c r="D153" s="18" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E153" s="21"/>
     </row>
@@ -4060,18 +4043,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
-    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100360305CF8A5F8A4B86568FB88F41EB51" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="7820bdd98b12bbce6701f392baa49827">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xmlns:ns3="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a7208ee71179b2cd86960a83168177e" ns2:_="" ns3:_="">
     <xsd:import namespace="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
@@ -4312,6 +4283,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
+    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4322,17 +4305,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C116F8E2-4DBC-4DB4-825C-1F8126BA2EE0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
-    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFB0FD70-63EF-4D48-A8C4-DFC9646D4D60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4351,6 +4323,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C116F8E2-4DBC-4DB4-825C-1F8126BA2EE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
+    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FD1144D-069D-4B6F-AEE5-711B319AB663}">
   <ds:schemaRefs>

</xml_diff>